<commit_message>
add mindMap and add some tables for bd proj
</commit_message>
<xml_diff>
--- a/BdProject.xlsx
+++ b/BdProject.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="схема БД" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
-  <si>
-    <t>CongratulationUser</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -53,9 +51,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>Congratulation</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
@@ -63,6 +58,54 @@
   </si>
   <si>
     <t>FromUserName</t>
+  </si>
+  <si>
+    <t>cu_CongratulationUser</t>
+  </si>
+  <si>
+    <t>cu_Gift</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>AnnotationText</t>
+  </si>
+  <si>
+    <t>cu_CongratulationCard</t>
+  </si>
+  <si>
+    <t>cu_UserCard</t>
+  </si>
+  <si>
+    <t>cu_CongratulationUserID</t>
+  </si>
+  <si>
+    <t>cu_CongratulationCardID</t>
+  </si>
+  <si>
+    <t>cu_UserGift</t>
+  </si>
+  <si>
+    <t>cu_GiftID</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cu_Photo</t>
+  </si>
+  <si>
+    <t>PhotoUrl</t>
+  </si>
+  <si>
+    <t>PhotoText</t>
+  </si>
+  <si>
+    <t>пользователь регистрируется</t>
+  </si>
+  <si>
+    <t>создаёт поздравительную открытку по шаблону</t>
   </si>
 </sst>
 </file>
@@ -381,84 +424,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>